<commit_message>
Integración con Google Sheets y soporte para Render
</commit_message>
<xml_diff>
--- a/cotizaciones.xlsx
+++ b/cotizaciones.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="73">
   <si>
     <t>FECHA REGISTRO</t>
   </si>
@@ -218,6 +218,18 @@
   </si>
   <si>
     <t>23:00</t>
+  </si>
+  <si>
+    <t>02/01/2026 22:52:25</t>
+  </si>
+  <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>02/01/2026 22:55:04</t>
+  </si>
+  <si>
+    <t>2026-01-31</t>
   </si>
 </sst>
 </file>
@@ -655,7 +667,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1487,6 +1499,166 @@
         <v>2499</v>
       </c>
     </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="3">
+        <v>26</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W11" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X11" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="3">
+        <v>26</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W12" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X12" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>3199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Agregar sistema de links para mensajes de cotización y corregir redirección a página de éxito
</commit_message>
<xml_diff>
--- a/cotizaciones.xlsx
+++ b/cotizaciones.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="91">
   <si>
     <t>FECHA REGISTRO</t>
   </si>
@@ -230,6 +230,60 @@
   </si>
   <si>
     <t>2026-01-31</t>
+  </si>
+  <si>
+    <t>03/01/2026 13:30:30</t>
+  </si>
+  <si>
+    <t>2026-02-08</t>
+  </si>
+  <si>
+    <t>04:30</t>
+  </si>
+  <si>
+    <t>San Miguel, La Cisterna, Región Metropolitana de Santiago 7970000, Chile</t>
+  </si>
+  <si>
+    <t>15.62</t>
+  </si>
+  <si>
+    <t>03/01/2026 13:37:20</t>
+  </si>
+  <si>
+    <t>03/01/2026 13:39:29</t>
+  </si>
+  <si>
+    <t>03/01/2026 13:50:05</t>
+  </si>
+  <si>
+    <t>03/01/2026 13:57:23</t>
+  </si>
+  <si>
+    <t>03/01/2026 14:05:11</t>
+  </si>
+  <si>
+    <t>03/01/2026 14:09:36</t>
+  </si>
+  <si>
+    <t>03/01/2026 14:14:58</t>
+  </si>
+  <si>
+    <t>2026-01-22</t>
+  </si>
+  <si>
+    <t>03/01/2026 14:17:41</t>
+  </si>
+  <si>
+    <t>2026-01-16</t>
+  </si>
+  <si>
+    <t>03/01/2026 14:19:00</t>
+  </si>
+  <si>
+    <t>03/01/2026 14:20:31</t>
+  </si>
+  <si>
+    <t>2026-01-29</t>
   </si>
 </sst>
 </file>
@@ -667,7 +721,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1659,6 +1713,886 @@
         <v>3199</v>
       </c>
     </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" s="3">
+        <v>25</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W13" s="5">
+        <v>33990</v>
+      </c>
+      <c r="X13" s="5">
+        <v>30591</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>3399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="3">
+        <v>29</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X14" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="3">
+        <v>29</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W15" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X15" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="3">
+        <v>28</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W16" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X16" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="3">
+        <v>28</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W17" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X17" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" s="3">
+        <v>28</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W18" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X18" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="3">
+        <v>28</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W19" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X19" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="3">
+        <v>28</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W20" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X20" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" s="3">
+        <v>29</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W21" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X21" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z21" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" s="3">
+        <v>29</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W22" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X22" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" s="3">
+        <v>29</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W23" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X23" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>3199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Actualizar cotizaciones de prueba con nuevo sistema de mensajes
</commit_message>
<xml_diff>
--- a/cotizaciones.xlsx
+++ b/cotizaciones.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="99">
   <si>
     <t>FECHA REGISTRO</t>
   </si>
@@ -284,6 +284,30 @@
   </si>
   <si>
     <t>2026-01-29</t>
+  </si>
+  <si>
+    <t>03/01/2026 16:42:49</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>Pacul, La Florida, Región Metropolitana de Santiago 8240000, Chile</t>
+  </si>
+  <si>
+    <t>Peñalolén, Región Metropolitana de Santiago, Chile</t>
+  </si>
+  <si>
+    <t>14.93</t>
+  </si>
+  <si>
+    <t>03/01/2026 16:48:19</t>
+  </si>
+  <si>
+    <t>03/01/2026 16:58:19</t>
+  </si>
+  <si>
+    <t>12.94</t>
   </si>
 </sst>
 </file>
@@ -721,7 +745,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2593,6 +2617,246 @@
         <v>3199</v>
       </c>
     </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O24" s="3">
+        <v>27</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W24" s="5">
+        <v>32990</v>
+      </c>
+      <c r="X24" s="5">
+        <v>29691</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z24" s="5">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O25" s="3">
+        <v>27</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W25" s="5">
+        <v>32990</v>
+      </c>
+      <c r="X25" s="5">
+        <v>29691</v>
+      </c>
+      <c r="Y25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z25" s="5">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" s="3">
+        <v>26</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W26" s="5">
+        <v>31990</v>
+      </c>
+      <c r="X26" s="5">
+        <v>28791</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z26" s="5">
+        <v>3199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>